<commit_message>
Updated POM.xml with latest version jar
</commit_message>
<xml_diff>
--- a/src/main/java/com/sayem/data/Test Cases.xlsx
+++ b/src/main/java/com/sayem/data/Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>TCID</t>
   </si>
@@ -39,39 +39,6 @@
   </si>
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>FindFriend</t>
-  </si>
-  <si>
-    <t>FriendName</t>
-  </si>
-  <si>
-    <t>PassWordChange</t>
-  </si>
-  <si>
-    <t>OldPassword</t>
-  </si>
-  <si>
-    <t>NewPassoword</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>D</t>
   </si>
   <si>
     <t>Data_Flag</t>
@@ -225,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -240,9 +207,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -550,7 +514,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +545,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
@@ -590,7 +554,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
@@ -599,7 +563,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
@@ -608,7 +572,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
@@ -617,7 +581,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
@@ -632,10 +596,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,10 +638,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -688,114 +652,18 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
Modified bunch of stuff
</commit_message>
<xml_diff>
--- a/src/main/java/com/sayem/data/Test Cases.xlsx
+++ b/src/main/java/com/sayem/data/Test Cases.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="19760" windowHeight="11560"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19755" windowHeight="11565"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -555,16 +555,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="2" width="18.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -575,7 +576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -584,7 +585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
@@ -593,7 +594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -602,7 +603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
@@ -611,7 +612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
@@ -620,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
@@ -648,16 +649,16 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="17.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -665,7 +666,7 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -679,7 +680,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -693,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -707,19 +708,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="12"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -727,26 +728,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -757,7 +758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -768,7 +769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -779,7 +780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -790,7 +791,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>